<commit_message>
Inserimento in file snapshot prime tabelle di test
</commit_message>
<xml_diff>
--- a/CONDIVISI/Configurazioni/Snapshot.xlsx
+++ b/CONDIVISI/Configurazioni/Snapshot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbasilico\Desktop\file_caricamento\CONDIVISI\Configurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EE1CFF-0127-469B-AE27-8B78B9F48766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ED5881-227C-4081-A974-84A7CF525631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22935" yWindow="825" windowWidth="14775" windowHeight="13230" xr2:uid="{C2A60027-5977-4507-A25B-158DE4796371}"/>
+    <workbookView xWindow="-28260" yWindow="1470" windowWidth="24570" windowHeight="13230" xr2:uid="{C2A60027-5977-4507-A25B-158DE4796371}"/>
   </bookViews>
   <sheets>
     <sheet name="Snapshot" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>database</t>
   </si>
@@ -88,23 +88,47 @@
     <t>LEGENDA FLUSSO</t>
   </si>
   <si>
-    <t>CRV</t>
-  </si>
-  <si>
-    <t>TARIFFARIO_XE</t>
-  </si>
-  <si>
-    <t>RFCF_CASHFLOW</t>
-  </si>
-  <si>
-    <t>RFCF_FATTURATO</t>
+    <t>rfcf_cashflow</t>
+  </si>
+  <si>
+    <t>rfcf_fatturato</t>
+  </si>
+  <si>
+    <t>crv</t>
+  </si>
+  <si>
+    <t>tariffario_xe</t>
+  </si>
+  <si>
+    <t>curato</t>
+  </si>
+  <si>
+    <t>netdo_codici_iva</t>
+  </si>
+  <si>
+    <t>tcr01_forniture_gas</t>
+  </si>
+  <si>
+    <t>xegy1_schede_tecniche_gas</t>
+  </si>
+  <si>
+    <t>dat_startDate</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>data.storico_xegy1_schede_tecniche_gas</t>
+  </si>
+  <si>
+    <t>Ricordarsi di inserire anche il nome del db in cui scrivere la tabella</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +143,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF555555"/>
+      <name val="Source Code Pro"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -147,11 +177,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -468,19 +502,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F264DCE-3DF0-4009-A241-257AD3B63836}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="37.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.44140625" customWidth="1"/>
     <col min="11" max="11" width="53.21875" customWidth="1"/>
   </cols>
@@ -512,6 +549,18 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
       <c r="J2" s="3" t="s">
         <v>3</v>
       </c>
@@ -519,6 +568,24 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
       <c r="J3" s="2" t="s">
         <v>4</v>
       </c>
@@ -527,6 +594,21 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
       <c r="J4" s="2" t="s">
         <v>5</v>
       </c>
@@ -550,22 +632,23 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E10" s="4"/>
+      <c r="J10" s="2" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J10" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J11" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -574,11 +657,18 @@
       </c>
       <c r="K13" s="3"/>
     </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J14:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correzione conti_clienti_day in cliente
</commit_message>
<xml_diff>
--- a/CONDIVISI/Configurazioni/Snapshot.xlsx
+++ b/CONDIVISI/Configurazioni/Snapshot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmascape\Documents\GitHub\databricks_provvisoria\file_caricamento\CONDIVISI\Configurazioni\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbasilico\Desktop\file_caricamento\CONDIVISI\Configurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ADE63C-58B2-46B7-A701-66B2273DA54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C5A831-0AA2-486A-813B-35489513EB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C2A60027-5977-4507-A25B-158DE4796371}"/>
+    <workbookView xWindow="9600" yWindow="600" windowWidth="17880" windowHeight="14220" xr2:uid="{C2A60027-5977-4507-A25B-158DE4796371}"/>
   </bookViews>
   <sheets>
     <sheet name="Snapshot" sheetId="1" r:id="rId1"/>
@@ -166,9 +166,6 @@
     <t>clcri_distributori</t>
   </si>
   <si>
-    <t>netdo_conti_clienti_day</t>
-  </si>
-  <si>
     <t>netdo_blocchi_fatturazione</t>
   </si>
   <si>
@@ -278,6 +275,9 @@
   </si>
   <si>
     <t>netdo_conti_cliente_bi</t>
+  </si>
+  <si>
+    <t>netdo_conti_cliente_day</t>
   </si>
 </sst>
 </file>
@@ -695,26 +695,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F264DCE-3DF0-4009-A241-257AD3B63836}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="59.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="53.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" customWidth="1"/>
+    <col min="11" max="11" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -741,7 +741,7 @@
       </c>
       <c r="I1" s="9"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -765,7 +765,7 @@
       <c r="K2" s="10"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
@@ -787,7 +787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -809,7 +809,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -828,7 +828,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -851,7 +851,7 @@
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -874,7 +874,7 @@
       </c>
       <c r="K7" s="11"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -893,7 +893,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -912,7 +912,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -931,7 +931,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -950,7 +950,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -969,7 +969,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -988,7 +988,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -1007,7 +1007,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1026,7 +1026,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1045,7 +1045,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -1064,7 +1064,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
@@ -1083,7 +1083,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>14</v>
       </c>
@@ -1100,11 +1100,11 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I19" s="8"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>4</v>
@@ -1123,7 +1123,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="8"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>4</v>
@@ -1142,7 +1142,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>4</v>
@@ -1161,7 +1161,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>6</v>
@@ -1178,11 +1178,11 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>4</v>
@@ -1201,7 +1201,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="8"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>17</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>4</v>
@@ -1220,7 +1220,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="8"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>17</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>4</v>
@@ -1239,7 +1239,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>17</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>4</v>
@@ -1258,7 +1258,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>17</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>5</v>
@@ -1281,7 +1281,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>14</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>17</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>5</v>
@@ -1304,7 +1304,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="8"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>14</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>17</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>5</v>
@@ -1327,7 +1327,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="8"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>14</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>17</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>5</v>
@@ -1350,7 +1350,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="8"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>14</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>17</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>5</v>
@@ -1373,7 +1373,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="8"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>17</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>5</v>
@@ -1396,7 +1396,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="8"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>14</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>17</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>5</v>
@@ -1419,7 +1419,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="8"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>14</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>17</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>5</v>
@@ -1442,7 +1442,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="8"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>14</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>17</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>5</v>
@@ -1465,7 +1465,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="8"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>17</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>5</v>
@@ -1488,7 +1488,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="8"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>14</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>17</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>5</v>
@@ -1511,7 +1511,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>14</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>17</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>5</v>
@@ -1534,7 +1534,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="8"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>14</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>17</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>6</v>
@@ -1551,11 +1551,11 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>14</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>17</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>6</v>
@@ -1572,11 +1572,11 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I41" s="8"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>14</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>17</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>6</v>
@@ -1593,11 +1593,11 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>16</v>
       </c>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="I43" s="8"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>17</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>4</v>
@@ -1637,7 +1637,7 @@
       <c r="H44" s="3"/>
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>14</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>17</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>6</v>
@@ -1654,11 +1654,11 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I45" s="8"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>14</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>17</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>6</v>
@@ -1675,11 +1675,11 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I46" s="8"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>14</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>17</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>6</v>
@@ -1696,11 +1696,11 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I47" s="8"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>14</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>17</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>6</v>
@@ -1717,11 +1717,11 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I48" s="8"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>14</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>17</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Aggiunta tabelle crv in file snapshot
</commit_message>
<xml_diff>
--- a/CONDIVISI/Configurazioni/Snapshot.xlsx
+++ b/CONDIVISI/Configurazioni/Snapshot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbasilico\Desktop\file_caricamento\CONDIVISI\Configurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C5A831-0AA2-486A-813B-35489513EB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EF86C1-ECB3-42EA-B9A0-44419638D992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="600" windowWidth="17880" windowHeight="14220" xr2:uid="{C2A60027-5977-4507-A25B-158DE4796371}"/>
+    <workbookView xWindow="11988" yWindow="2220" windowWidth="28680" windowHeight="14220" xr2:uid="{C2A60027-5977-4507-A25B-158DE4796371}"/>
   </bookViews>
   <sheets>
     <sheet name="Snapshot" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="80">
   <si>
     <t>database</t>
   </si>
@@ -693,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F264DCE-3DF0-4009-A241-257AD3B63836}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1740,6 +1740,144 @@
       <c r="H49" s="3"/>
       <c r="I49" s="8"/>
     </row>
+    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="8"/>
+    </row>
+    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="8"/>
+    </row>
+    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="8"/>
+    </row>
+    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="8"/>
+    </row>
+    <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="8"/>
+    </row>
+    <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="8"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="J2:K2"/>

</xml_diff>

<commit_message>
Inserimento file input RFCF_fatturato in snapshot
</commit_message>
<xml_diff>
--- a/CONDIVISI/Configurazioni/Snapshot.xlsx
+++ b/CONDIVISI/Configurazioni/Snapshot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbasilico\Desktop\file_caricamento\CONDIVISI\Configurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8099B4C-A29F-4D30-8A04-D4533BF3162B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A0B59D-09D2-4CA5-A059-A97DC48BE7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11292" yWindow="1524" windowWidth="28680" windowHeight="14220" xr2:uid="{C2A60027-5977-4507-A25B-158DE4796371}"/>
+    <workbookView xWindow="2844" yWindow="1236" windowWidth="33408" windowHeight="14220" xr2:uid="{C2A60027-5977-4507-A25B-158DE4796371}"/>
   </bookViews>
   <sheets>
     <sheet name="Snapshot" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="98">
   <si>
     <t>database</t>
   </si>
@@ -278,6 +278,60 @@
   </si>
   <si>
     <t>tcr01_cambio_prodotto</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>rfcf_configurazione_start_run</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>tcr_configurazione_storico_snapshot</t>
+  </si>
+  <si>
+    <t>tcr_decodifiche</t>
+  </si>
+  <si>
+    <t>tcr_codifiche_tariffario</t>
+  </si>
+  <si>
+    <t>tcr_mapping_xe_gas</t>
+  </si>
+  <si>
+    <t>tcr_mapping_xe_pwr</t>
+  </si>
+  <si>
+    <t>tcr_tariffario_xe_indici_fatturazione</t>
+  </si>
+  <si>
+    <t>rfcf_calendario_fatturazione_mensile_all_ver</t>
+  </si>
+  <si>
+    <t>rfcf_calendario_xe_date</t>
+  </si>
+  <si>
+    <t>rfcf_calendario_xe_forn</t>
+  </si>
+  <si>
+    <t>rfcf_estrazione_CE</t>
+  </si>
+  <si>
+    <t>rfcf_estrazione_DR</t>
+  </si>
+  <si>
+    <t>rfcf_parametri_previsione_extra</t>
+  </si>
+  <si>
+    <t>rfcf_forzatura_iva</t>
+  </si>
+  <si>
+    <t>rfcf_ordine_default_tioce</t>
+  </si>
+  <si>
+    <t>rfcf_tipo_regime</t>
   </si>
 </sst>
 </file>
@@ -693,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F264DCE-3DF0-4009-A241-257AD3B63836}">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1878,6 +1932,294 @@
       <c r="H55" s="3"/>
       <c r="I55" s="8"/>
     </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="J2:K2"/>

</xml_diff>

<commit_message>
modifica snapshot con fcf2
</commit_message>
<xml_diff>
--- a/CONDIVISI/Configurazioni/Snapshot.xlsx
+++ b/CONDIVISI/Configurazioni/Snapshot.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbasilico\Desktop\file_caricamento\CONDIVISI\Configurazioni\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmascape\Documents\GitHub\databricks_provvisoria\file_caricamento\CONDIVISI\Configurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A0B59D-09D2-4CA5-A059-A97DC48BE7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA0E779-2B0A-408B-8934-3EE7D6B00CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2844" yWindow="1236" windowWidth="33408" windowHeight="14220" xr2:uid="{C2A60027-5977-4507-A25B-158DE4796371}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C2A60027-5977-4507-A25B-158DE4796371}"/>
   </bookViews>
   <sheets>
     <sheet name="Snapshot" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Snapshot!$C$1:$C$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Snapshot!$A$1:$H$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="102">
   <si>
     <t>database</t>
   </si>
@@ -332,6 +332,18 @@
   </si>
   <si>
     <t>rfcf_tipo_regime</t>
+  </si>
+  <si>
+    <t>rfcf_storico_run_cashflow</t>
+  </si>
+  <si>
+    <t>rfcf_configurazione_start_run_cashflow</t>
+  </si>
+  <si>
+    <t>rfcf_decodifiche_cashflow</t>
+  </si>
+  <si>
+    <t>rfcf_parametri_check_decodifiche</t>
   </si>
 </sst>
 </file>
@@ -747,28 +759,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F264DCE-3DF0-4009-A241-257AD3B63836}">
-  <dimension ref="A1:L71"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="59.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" customWidth="1"/>
-    <col min="11" max="11" width="53.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="53.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -795,7 +807,7 @@
       </c>
       <c r="I1" s="9"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -819,7 +831,7 @@
       <c r="K2" s="10"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
@@ -841,7 +853,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -863,7 +875,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -882,7 +894,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -905,7 +917,7 @@
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -928,7 +940,7 @@
       </c>
       <c r="K7" s="11"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -947,7 +959,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -966,7 +978,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -985,7 +997,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -1004,7 +1016,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -1023,7 +1035,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1042,7 +1054,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -1061,7 +1073,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1080,7 +1092,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1099,7 +1111,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -1118,7 +1130,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
@@ -1137,7 +1149,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>14</v>
       </c>
@@ -1158,7 +1170,7 @@
       </c>
       <c r="I19" s="8"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -1177,7 +1189,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="8"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
@@ -1196,7 +1208,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
@@ -1215,7 +1227,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -1236,7 +1248,7 @@
       </c>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -1255,7 +1267,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="8"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
@@ -1274,7 +1286,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="8"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -1293,7 +1305,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
@@ -1312,7 +1324,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
@@ -1335,7 +1347,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>14</v>
       </c>
@@ -1358,7 +1370,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="8"/>
     </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>14</v>
       </c>
@@ -1381,7 +1393,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="8"/>
     </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>14</v>
       </c>
@@ -1404,7 +1416,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="8"/>
     </row>
-    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>14</v>
       </c>
@@ -1427,7 +1439,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="8"/>
     </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
@@ -1450,7 +1462,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="8"/>
     </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>14</v>
       </c>
@@ -1473,7 +1485,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="8"/>
     </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>14</v>
       </c>
@@ -1496,7 +1508,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="8"/>
     </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>14</v>
       </c>
@@ -1519,7 +1531,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="8"/>
     </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
@@ -1542,7 +1554,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="8"/>
     </row>
-    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>14</v>
       </c>
@@ -1565,7 +1577,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>14</v>
       </c>
@@ -1588,7 +1600,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="8"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>14</v>
       </c>
@@ -1609,7 +1621,7 @@
       </c>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>14</v>
       </c>
@@ -1630,7 +1642,7 @@
       </c>
       <c r="I41" s="8"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>14</v>
       </c>
@@ -1651,7 +1663,7 @@
       </c>
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>16</v>
       </c>
@@ -1672,7 +1684,7 @@
       </c>
       <c r="I43" s="8"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -1691,7 +1703,7 @@
       <c r="H44" s="3"/>
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>14</v>
       </c>
@@ -1712,7 +1724,7 @@
       </c>
       <c r="I45" s="8"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>14</v>
       </c>
@@ -1733,7 +1745,7 @@
       </c>
       <c r="I46" s="8"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>14</v>
       </c>
@@ -1754,7 +1766,7 @@
       </c>
       <c r="I47" s="8"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>14</v>
       </c>
@@ -1775,7 +1787,7 @@
       </c>
       <c r="I48" s="8"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>14</v>
       </c>
@@ -1794,7 +1806,7 @@
       <c r="H49" s="3"/>
       <c r="I49" s="8"/>
     </row>
-    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>15</v>
       </c>
@@ -1817,7 +1829,7 @@
       <c r="H50" s="3"/>
       <c r="I50" s="8"/>
     </row>
-    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>15</v>
       </c>
@@ -1840,7 +1852,7 @@
       <c r="H51" s="3"/>
       <c r="I51" s="8"/>
     </row>
-    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>15</v>
       </c>
@@ -1863,7 +1875,7 @@
       <c r="H52" s="3"/>
       <c r="I52" s="8"/>
     </row>
-    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>15</v>
       </c>
@@ -1886,7 +1898,7 @@
       <c r="H53" s="3"/>
       <c r="I53" s="8"/>
     </row>
-    <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>15</v>
       </c>
@@ -1909,7 +1921,7 @@
       <c r="H54" s="3"/>
       <c r="I54" s="8"/>
     </row>
-    <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>15</v>
       </c>
@@ -1932,7 +1944,7 @@
       <c r="H55" s="3"/>
       <c r="I55" s="8"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>14</v>
       </c>
@@ -1950,7 +1962,7 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>14</v>
       </c>
@@ -1968,7 +1980,7 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>14</v>
       </c>
@@ -1986,7 +1998,7 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>14</v>
       </c>
@@ -2004,7 +2016,7 @@
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>14</v>
       </c>
@@ -2022,7 +2034,7 @@
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>14</v>
       </c>
@@ -2040,7 +2052,7 @@
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>14</v>
       </c>
@@ -2058,7 +2070,7 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>14</v>
       </c>
@@ -2076,7 +2088,7 @@
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>14</v>
       </c>
@@ -2094,7 +2106,7 @@
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>14</v>
       </c>
@@ -2112,7 +2124,7 @@
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>14</v>
       </c>
@@ -2130,7 +2142,7 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>14</v>
       </c>
@@ -2148,7 +2160,7 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>14</v>
       </c>
@@ -2166,7 +2178,7 @@
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>14</v>
       </c>
@@ -2184,7 +2196,7 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>14</v>
       </c>
@@ -2202,7 +2214,7 @@
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>14</v>
       </c>
@@ -2220,7 +2232,80 @@
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
     </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:H74" xr:uid="{9F264DCE-3DF0-4009-A241-257AD3B63836}"/>
   <mergeCells count="3">
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="J6:K6"/>

</xml_diff>